<commit_message>
updated order detail for BDCLC controllers, received working controllers from JLC
</commit_message>
<xml_diff>
--- a/MP6532_board_28-QFN/assembly/MP6532_board_28-QFN-2.xlsx
+++ b/MP6532_board_28-QFN/assembly/MP6532_board_28-QFN-2.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">C48974</t>
   </si>
   <si>
-    <t xml:space="preserve">470nF/100V</t>
+    <t xml:space="preserve">470nF/100V (not available on order C97926 )</t>
   </si>
   <si>
     <t xml:space="preserve">C15</t>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">C_0805_2012Metric</t>
   </si>
   <si>
-    <t xml:space="preserve">C97926</t>
+    <t xml:space="preserve">C16195147</t>
   </si>
   <si>
     <t xml:space="preserve">4.7uF</t>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">C 100nF</t>
   </si>
   <si>
-    <t xml:space="preserve">C17,C19,C18,C7,C8,C9</t>
+    <t xml:space="preserve">C17,C19,C18,C7,C8,C9,C10,C11,C12</t>
   </si>
   <si>
     <t xml:space="preserve">C_0603_1608Metric</t>
@@ -136,7 +136,23 @@
     <t xml:space="preserve">C21190</t>
   </si>
   <si>
-    <t xml:space="preserve">LED RED</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">LED RED (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">C2295 not available on order)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">D7</t>
@@ -145,7 +161,7 @@
     <t xml:space="preserve">LED_0805_2012Metric</t>
   </si>
   <si>
-    <t xml:space="preserve">C2295</t>
+    <t xml:space="preserve">C965812</t>
   </si>
   <si>
     <t xml:space="preserve">LED BLUE</t>
@@ -160,13 +176,13 @@
     <t xml:space="preserve">Res 10K</t>
   </si>
   <si>
-    <t xml:space="preserve">R8,R9,R10,R11,R12,R13</t>
+    <t xml:space="preserve">R8,R9,R10,R11,R12,R13,R25,R26,R27</t>
   </si>
   <si>
     <t xml:space="preserve">C25804</t>
   </si>
   <si>
-    <t xml:space="preserve">MP6532</t>
+    <t xml:space="preserve">MP6532 from My parts / digikey 1589-MP6532GR-ZCT-ND </t>
   </si>
   <si>
     <t xml:space="preserve">U1</t>
@@ -197,11 +213,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -220,6 +237,12 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -296,12 +319,12 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="65.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.52"/>

</xml_diff>